<commit_message>
synch commit for refreshing the repo
</commit_message>
<xml_diff>
--- a/dtpu_configurations/only_integer8/mxu_10x10_30mhz/timing.xlsx
+++ b/dtpu_configurations/only_integer8/mxu_10x10_30mhz/timing.xlsx
@@ -119,10 +119,10 @@
         <v>3</v>
       </c>
       <c r="B2" t="n" s="4">
-        <v>16.832040786743164</v>
+        <v>17.5273494720459</v>
       </c>
       <c r="C2" t="n" s="4">
-        <v>0.019001023843884468</v>
+        <v>0.007638223469257355</v>
       </c>
     </row>
   </sheetData>

</xml_diff>